<commit_message>
email function work but trying to improve vendors regex
</commit_message>
<xml_diff>
--- a/vendors_list.xlsx
+++ b/vendors_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8e402ea66b88ec45/Documents/Python Projects/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Python Projects\VulnMonitor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="11_F25DC773A252ABDACC1048BEB91C54425ADE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6608AE1A-165A-4572-ADD7-FDA63278684F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0742147A-E7FB-4AAE-AE4A-ABA740AB9DDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57495" yWindow="10980" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Microsoft</t>
   </si>
@@ -46,6 +46,18 @@
   </si>
   <si>
     <t>MICROSENS</t>
+  </si>
+  <si>
+    <t>MagLink</t>
+  </si>
+  <si>
+    <t>MikoPBX</t>
+  </si>
+  <si>
+    <t>eosphoros-ai</t>
+  </si>
+  <si>
+    <t>HKUDS</t>
   </si>
 </sst>
 </file>
@@ -98,10 +110,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -367,15 +375,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
@@ -413,7 +421,28 @@
         <v>6</v>
       </c>
     </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
improved vendor keyword done
</commit_message>
<xml_diff>
--- a/vendors_list.xlsx
+++ b/vendors_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Python Projects\VulnMonitor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0742147A-E7FB-4AAE-AE4A-ABA740AB9DDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17757CC8-A6B8-4475-88BC-EC38C4FA0641}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57495" yWindow="10980" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="76695" yWindow="10980" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Microsoft</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>HKUDS</t>
+  </si>
+  <si>
+    <t>wpnb_pto_new_users_add()</t>
   </si>
 </sst>
 </file>
@@ -375,15 +378,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="F18" sqref="F17:F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.36328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
@@ -441,6 +444,11 @@
         <v>10</v>
       </c>
     </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
writing and reading nvdcve-1.1-recent.json is not not needed
</commit_message>
<xml_diff>
--- a/vendors_list.xlsx
+++ b/vendors_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Python Projects\VulnMonitor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7846608-4CDE-4A9D-A5BB-3509F1E41BF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40DCC840-28C8-485F-BB62-84FADC7C46B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57345" yWindow="14070" windowWidth="24840" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="61380" yWindow="18705" windowWidth="24840" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Microsoft</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>POP</t>
+  </si>
+  <si>
+    <t>zuluCrypt</t>
   </si>
 </sst>
 </file>
@@ -390,10 +393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A13"/>
+  <dimension ref="A1:A14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -466,6 +469,11 @@
         <v>12</v>
       </c>
     </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
changed how the number of days is coded
</commit_message>
<xml_diff>
--- a/vendors_list.xlsx
+++ b/vendors_list.xlsx
@@ -8,24 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Python Projects\VulnMonitor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40DCC840-28C8-485F-BB62-84FADC7C46B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66B697E8-49AF-4F0C-BB5E-3FEA908F367B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="61380" yWindow="18705" windowWidth="24840" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="76695" yWindow="10980" windowWidth="19395" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Microsoft</t>
   </si>
@@ -61,12 +72,6 @@
   </si>
   <si>
     <t>wpnb_pto_new_users_add()</t>
-  </si>
-  <si>
-    <t>POP</t>
-  </si>
-  <si>
-    <t>zuluCrypt</t>
   </si>
 </sst>
 </file>
@@ -396,7 +401,7 @@
   <dimension ref="A1:A14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -465,14 +470,10 @@
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="A13" s="1"/>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A14" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="A14" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>